<commit_message>
prepare for jit, indexing cleanup
</commit_message>
<xml_diff>
--- a/in/2cam_flame.xlsx
+++ b/in/2cam_flame.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sim" sheetId="1" state="visible" r:id="rId2"/>
@@ -255,7 +255,7 @@
     <author/>
   </authors>
   <commentList>
-    <comment ref="A8" authorId="0">
+    <comment ref="A7" authorId="0">
       <text>
         <r>
           <rPr>
@@ -272,7 +272,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A9" authorId="0">
+    <comment ref="A8" authorId="0">
       <text>
         <r>
           <rPr>
@@ -293,7 +293,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="133">
   <si>
     <t>Sim</t>
   </si>
@@ -355,7 +355,7 @@
     <t>TranscarDataDir</t>
   </si>
   <si>
-    <t>~/U/transcar/out/gfortran</t>
+    <t>~/code/transcar/out/ifort</t>
   </si>
   <si>
     <t>ExcitationDATfn</t>
@@ -641,9 +641,6 @@
   </si>
   <si>
     <t>Arc4</t>
-  </si>
-  <si>
-    <t>useArc</t>
   </si>
   <si>
     <t>X0km</t>
@@ -1003,7 +1000,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="61">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1248,10 +1245,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1333,9 +1326,9 @@
   <dimension ref="A1:H65536"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="D45" activeCellId="0" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -1817,7 +1810,7 @@
       <c r="B44" s="0"/>
       <c r="C44" s="0"/>
       <c r="D44" s="33" t="n">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="E44" s="34"/>
       <c r="F44" s="13"/>
@@ -9106,12 +9099,12 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G1" activeCellId="0" sqref="G1"/>
+      <selection pane="bottomLeft" activeCell="F26" activeCellId="0" sqref="F26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9139,10 +9132,10 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="4" t="s">
         <v>116</v>
       </c>
-      <c r="B2" s="61" t="n">
+      <c r="B2" s="4" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="0" t="n">
@@ -9162,21 +9155,7 @@
       <c r="A3" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="B3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="0" t="n">
-        <v>1</v>
-      </c>
+      <c r="B3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
@@ -9188,126 +9167,140 @@
       <c r="A5" s="4" t="s">
         <v>119</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="4" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="F5" s="0" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
         <v>120</v>
       </c>
       <c r="B6" s="4" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="C6" s="0" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="D6" s="0" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="E6" s="0" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="F6" s="0" t="n">
-        <v>0.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="B7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>1</v>
+      <c r="B7" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="B9" s="4" t="s">
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="C9" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>125</v>
+      <c r="B10" s="0" t="n">
+        <v>500</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>1000</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>2500</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>5000</v>
+      </c>
+      <c r="F10" s="0" t="n">
+        <v>10000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="0" t="s">
         <v>126</v>
       </c>
-      <c r="B11" s="0" t="n">
-        <v>500</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>2500</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>5000</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>10000</v>
+      <c r="B11" s="50" t="n">
+        <v>80000000000</v>
+      </c>
+      <c r="C11" s="50" t="n">
+        <v>225000000000</v>
+      </c>
+      <c r="D11" s="50" t="n">
+        <v>1000000000000</v>
+      </c>
+      <c r="E11" s="50" t="n">
+        <v>2800000000000</v>
+      </c>
+      <c r="F11" s="50" t="n">
+        <v>5000000000000</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="B12" s="50" t="n">
-        <v>80000000000</v>
-      </c>
-      <c r="C12" s="50" t="n">
-        <v>225000000000</v>
-      </c>
-      <c r="D12" s="50" t="n">
-        <v>1000000000000</v>
-      </c>
-      <c r="E12" s="50" t="n">
-        <v>2800000000000</v>
-      </c>
-      <c r="F12" s="50" t="n">
-        <v>5000000000000</v>
+      <c r="B12" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>0.375</v>
+      </c>
+      <c r="F12" s="0" t="n">
+        <v>0.25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9315,19 +9308,19 @@
         <v>128</v>
       </c>
       <c r="B13" s="0" t="n">
-        <v>1</v>
+        <v>0.8</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>0.75</v>
+        <v>0.8</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>0.5</v>
+        <v>0.8</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>0.375</v>
+        <v>0.8</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>0.25</v>
+        <v>0.8</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9335,19 +9328,19 @@
         <v>129</v>
       </c>
       <c r="B14" s="0" t="n">
-        <v>0.8</v>
+        <v>3</v>
       </c>
       <c r="C14" s="0" t="n">
-        <v>0.8</v>
+        <v>3</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>0.8</v>
+        <v>3</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>0.8</v>
+        <v>2.5</v>
       </c>
       <c r="F14" s="0" t="n">
-        <v>0.8</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9355,19 +9348,19 @@
         <v>130</v>
       </c>
       <c r="B15" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E15" s="0" t="n">
+        <v>3.5</v>
+      </c>
+      <c r="F15" s="0" t="n">
         <v>2.5</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <v>2</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9375,19 +9368,19 @@
         <v>131</v>
       </c>
       <c r="B16" s="0" t="n">
-        <v>4</v>
+        <v>900</v>
       </c>
       <c r="C16" s="0" t="n">
-        <v>4</v>
+        <v>3000</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>4</v>
+        <v>4000</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>3.5</v>
+        <v>10000</v>
       </c>
       <c r="F16" s="0" t="n">
-        <v>2.5</v>
+        <v>18000</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9395,38 +9388,18 @@
         <v>132</v>
       </c>
       <c r="B17" s="0" t="n">
-        <v>900</v>
+        <v>0.145</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>3000</v>
+        <v>0.15</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>4000</v>
+        <v>0.145</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>10000</v>
+        <v>0.2</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>18000</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="B18" s="0" t="n">
-        <v>0.145</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <v>0.145</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="F18" s="0" t="n">
         <v>0.6</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fwd scaling, need inv scaling
</commit_message>
<xml_diff>
--- a/in/2cam_flame.xlsx
+++ b/in/2cam_flame.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="986" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sim" sheetId="1" state="visible" r:id="rId2"/>
@@ -245,6 +245,19 @@
         </r>
       </text>
     </comment>
+    <comment ref="A44" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Photoelectron/data number</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
@@ -293,7 +306,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="130">
   <si>
     <t>Sim</t>
   </si>
@@ -628,19 +641,10 @@
     <t>hst1cal.h5</t>
   </si>
   <si>
-    <t>Arc0</t>
-  </si>
-  <si>
-    <t>Arc1</t>
-  </si>
-  <si>
-    <t>Arc2</t>
-  </si>
-  <si>
-    <t>Arc3</t>
-  </si>
-  <si>
-    <t>Arc4</t>
+    <t>pixarea_m</t>
+  </si>
+  <si>
+    <t>pedn</t>
   </si>
   <si>
     <t>X0km</t>
@@ -698,11 +702,12 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="164" formatCode="GENERAL"/>
     <numFmt numFmtId="165" formatCode="@"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
-    <numFmt numFmtId="167" formatCode="0.00E+000"/>
+    <numFmt numFmtId="167" formatCode="0"/>
+    <numFmt numFmtId="168" formatCode="0.00E+000"/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -1000,7 +1005,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="63">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1245,6 +1250,14 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="168" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
@@ -1974,12 +1987,12 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IR41"/>
+  <dimension ref="A1:IR44"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="bottomLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -4074,10 +4087,10 @@
         <v>80</v>
       </c>
       <c r="B9" s="50" t="n">
-        <v>100000000</v>
+        <v>100</v>
       </c>
       <c r="C9" s="50" t="n">
-        <v>100000000</v>
+        <v>100</v>
       </c>
       <c r="D9" s="0"/>
       <c r="E9" s="0"/>
@@ -4334,10 +4347,10 @@
         <v>81</v>
       </c>
       <c r="B10" s="50" t="n">
-        <v>100000000</v>
+        <v>100</v>
       </c>
       <c r="C10" s="50" t="n">
-        <v>100000000</v>
+        <v>100</v>
       </c>
       <c r="D10" s="0"/>
       <c r="E10" s="0"/>
@@ -5105,8 +5118,12 @@
       <c r="A13" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="B13" s="0"/>
-      <c r="C13" s="0"/>
+      <c r="B13" s="0" t="n">
+        <v>50</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>50</v>
+      </c>
       <c r="D13" s="0"/>
       <c r="E13" s="0"/>
       <c r="F13" s="0"/>
@@ -9081,6 +9098,28 @@
         <v>110</v>
       </c>
     </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="43" t="s">
+        <v>111</v>
+      </c>
+      <c r="B43" s="61" t="n">
+        <v>1.6E-005</v>
+      </c>
+      <c r="C43" s="61" t="n">
+        <v>1.6E-005</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="43" t="s">
+        <v>112</v>
+      </c>
+      <c r="B44" s="43" t="n">
+        <v>1</v>
+      </c>
+      <c r="C44" s="43" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="1" right="1" top="1.66666666666667" bottom="1.66666666666667" header="0.511805555555555" footer="0.511805555555555"/>
@@ -9099,12 +9138,12 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:H17"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="G17" activeCellId="0" sqref="G17"/>
+      <selection pane="bottomLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9115,30 +9154,36 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B1" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>113</v>
-      </c>
-      <c r="E1" s="0" t="s">
-        <v>114</v>
-      </c>
-      <c r="F1" s="0" t="s">
-        <v>115</v>
+      <c r="B1" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="0" t="n">
+        <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="C2" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D2" s="0" t="n">
@@ -9150,27 +9195,35 @@
       <c r="F2" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>0.5</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="C5" s="4" t="n">
         <v>0.5</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -9182,15 +9235,21 @@
       <c r="F5" s="0" t="n">
         <v>0.5</v>
       </c>
+      <c r="G5" s="0" t="n">
+        <v>0.5</v>
+      </c>
+      <c r="H5" s="0" t="n">
+        <v>0.5</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>1</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="C6" s="4" t="n">
         <v>1</v>
       </c>
       <c r="D6" s="0" t="n">
@@ -9202,110 +9261,146 @@
       <c r="F6" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="G6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="0" t="n">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>119</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>500</v>
       </c>
       <c r="C10" s="0" t="n">
+        <v>750</v>
+      </c>
+      <c r="D10" s="0" t="n">
         <v>1000</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="E10" s="0" t="n">
         <v>2500</v>
       </c>
-      <c r="E10" s="0" t="n">
+      <c r="F10" s="0" t="n">
+        <v>3750</v>
+      </c>
+      <c r="G10" s="0" t="n">
         <v>5000</v>
       </c>
-      <c r="F10" s="0" t="n">
+      <c r="H10" s="0" t="n">
         <v>10000</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="B11" s="50" t="n">
+        <v>123</v>
+      </c>
+      <c r="B11" s="62" t="n">
         <v>80000000000</v>
       </c>
-      <c r="C11" s="50" t="n">
+      <c r="C11" s="62" t="n">
+        <v>100000000000</v>
+      </c>
+      <c r="D11" s="62" t="n">
         <v>225000000000</v>
       </c>
-      <c r="D11" s="50" t="n">
+      <c r="E11" s="62" t="n">
         <v>500000000000</v>
       </c>
-      <c r="E11" s="50" t="n">
+      <c r="F11" s="62" t="n">
+        <v>700000000000</v>
+      </c>
+      <c r="G11" s="62" t="n">
         <v>900000000000</v>
       </c>
-      <c r="F11" s="50" t="n">
+      <c r="H11" s="62" t="n">
         <v>1100000000000</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>1</v>
       </c>
       <c r="C12" s="0" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="D12" s="0" t="n">
         <v>0.75</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="E12" s="0" t="n">
         <v>0.5</v>
       </c>
-      <c r="E12" s="0" t="n">
+      <c r="F12" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G12" s="0" t="n">
         <v>0.375</v>
       </c>
-      <c r="F12" s="0" t="n">
+      <c r="H12" s="0" t="n">
         <v>0.25</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.8</v>
@@ -9322,10 +9417,16 @@
       <c r="F13" s="0" t="n">
         <v>0.8</v>
       </c>
+      <c r="G13" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>0.8</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>3</v>
@@ -9334,18 +9435,24 @@
         <v>3</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>2.5</v>
+        <v>3</v>
       </c>
       <c r="E14" s="0" t="n">
         <v>2.5</v>
       </c>
       <c r="F14" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>2.5</v>
+      </c>
+      <c r="H14" s="0" t="n">
         <v>3</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>4</v>
@@ -9362,30 +9469,42 @@
       <c r="F15" s="0" t="n">
         <v>4</v>
       </c>
+      <c r="G15" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>4</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>900</v>
       </c>
       <c r="C16" s="0" t="n">
+        <v>1200</v>
+      </c>
+      <c r="D16" s="0" t="n">
         <v>3000</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="E16" s="0" t="n">
         <v>4000</v>
       </c>
-      <c r="E16" s="0" t="n">
+      <c r="F16" s="0" t="n">
+        <v>4750</v>
+      </c>
+      <c r="G16" s="0" t="n">
         <v>5500</v>
       </c>
-      <c r="F16" s="0" t="n">
+      <c r="H16" s="0" t="n">
         <v>7500</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>0.145</v>
@@ -9394,12 +9513,18 @@
         <v>0.15</v>
       </c>
       <c r="D17" s="0" t="n">
+        <v>0.15</v>
+      </c>
+      <c r="E17" s="0" t="n">
         <v>0.2</v>
       </c>
-      <c r="E17" s="0" t="n">
+      <c r="F17" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G17" s="0" t="n">
         <v>0.3</v>
       </c>
-      <c r="F17" s="0" t="n">
+      <c r="H17" s="0" t="n">
         <v>0.4</v>
       </c>
     </row>

</xml_diff>

<commit_message>
work to have multitimes and multiarc
</commit_message>
<xml_diff>
--- a/in/2cam_flame.xlsx
+++ b/in/2cam_flame.xlsx
@@ -5,12 +5,13 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="977" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sim" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Cameras" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Arcs" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Arc0" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Arc1" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="1" name="Excel_BuiltIn_Print_Area" vbProcedure="false">NA()</definedName>
@@ -320,7 +321,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="134">
   <si>
     <t>Sim</t>
   </si>
@@ -1355,12 +1356,12 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H65"/>
+  <dimension ref="A1:H79"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="E55" activeCellId="0" sqref="E55"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B79" activeCellId="1" sqref="C11:H18 B79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1873,7 +1874,7 @@
       <c r="G47" s="0"/>
       <c r="H47" s="0"/>
     </row>
-    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="31" t="s">
         <v>60</v>
       </c>
@@ -2035,6 +2036,7 @@
       </c>
       <c r="C65" s="5"/>
     </row>
+    <row r="79" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2058,7 +2060,7 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C24" activeCellId="0" sqref="C24"/>
+      <selection pane="bottomLeft" activeCell="C6" activeCellId="1" sqref="C11:H18 C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -3371,7 +3373,7 @@
         <v>90</v>
       </c>
       <c r="C6" s="46" t="n">
-        <v>88.3</v>
+        <v>88.0172525718237</v>
       </c>
       <c r="D6" s="0"/>
       <c r="E6" s="0"/>
@@ -9197,12 +9199,12 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H18"/>
+  <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
-      <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="B1" activeCellId="1" sqref="C11:H18 B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9236,7 +9238,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
         <v>116</v>
       </c>
@@ -9262,7 +9264,7 @@
         <v>0.12</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>117</v>
       </c>
@@ -9614,6 +9616,7 @@
         <v>0.145</v>
       </c>
     </row>
+    <row r="58" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -9624,4 +9627,433 @@
   </headerFooter>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:H18"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11:H18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.85"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="4"/>
+      <c r="B1" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C1" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D1" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E1" s="4" t="n">
+        <v>3</v>
+      </c>
+      <c r="F1" s="4" t="n">
+        <v>4</v>
+      </c>
+      <c r="G1" s="4" t="n">
+        <v>5</v>
+      </c>
+      <c r="H1" s="4" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="C2" s="61" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="D2" s="61" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="E2" s="61" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="F2" s="61" t="n">
+        <v>0.08</v>
+      </c>
+      <c r="G2" s="61" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="61" t="n">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="B3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="C3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="D3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" s="4" t="n">
+        <v>2</v>
+      </c>
+      <c r="H3" s="4" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="B6" s="4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="C6" s="4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="D6" s="4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="E6" s="4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="F6" s="4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="G6" s="4" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H6" s="4" t="n">
+        <v>0.1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="B7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="C7" s="4" t="n">
+        <v>1</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="F7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="H7" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="4" t="s">
+        <v>122</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="4" t="s">
+        <v>124</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="G11" s="0" t="n">
+        <v>10000</v>
+      </c>
+      <c r="H11" s="0" t="n">
+        <v>10000</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B12" s="62" t="n">
+        <v>1100000000000</v>
+      </c>
+      <c r="C12" s="62" t="n">
+        <v>1100000000000</v>
+      </c>
+      <c r="D12" s="62" t="n">
+        <v>1100000000000</v>
+      </c>
+      <c r="E12" s="62" t="n">
+        <v>1100000000000</v>
+      </c>
+      <c r="F12" s="62" t="n">
+        <v>1100000000000</v>
+      </c>
+      <c r="G12" s="62" t="n">
+        <v>1100000000000</v>
+      </c>
+      <c r="H12" s="62" t="n">
+        <v>1100000000000</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="F13" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G13" s="0" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="H13" s="0" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="F14" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="G14" s="0" t="n">
+        <v>0.8</v>
+      </c>
+      <c r="H14" s="0" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="G15" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="H15" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>131</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="F16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="G16" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="H16" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>7500</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>7500</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>7500</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>7500</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>7500</v>
+      </c>
+      <c r="G17" s="0" t="n">
+        <v>7500</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>7500</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="s">
+        <v>133</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="E18" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="F18" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="G18" s="0" t="n">
+        <v>0.4</v>
+      </c>
+      <c r="H18" s="0" t="n">
+        <v>0.4</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
overall offline analysis, maxwellian init option
</commit_message>
<xml_diff>
--- a/in/2cam_flame.xlsx
+++ b/in/2cam_flame.xlsx
@@ -5,13 +5,12 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sim" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Cameras" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Arc0" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Arc1" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName function="false" hidden="false" localSheetId="1" name="Excel_BuiltIn_Print_Area" vbProcedure="false">NA()</definedName>
@@ -145,7 +144,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A60" authorId="0">
+    <comment ref="A61" authorId="0">
       <text>
         <r>
           <rPr>
@@ -163,7 +162,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A65" authorId="0">
+    <comment ref="A66" authorId="0">
       <text>
         <r>
           <rPr>
@@ -277,51 +276,8 @@
 </comments>
 </file>
 
-<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
-  <authors>
-    <author/>
-  </authors>
-  <commentList>
-    <comment ref="A8" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Gaussian: gaussian horizontal shape
-Rect: boxcar horizontal shape
-Sinc2: Sinc(.)^2 horizontal shaping
-None: no smearing at all horizontally</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="A9" authorId="0">
-      <text>
-        <r>
-          <rPr>
-            <sz val="10"/>
-            <color rgb="FF000000"/>
-            <rFont val="Arial"/>
-            <family val="2"/>
-            <charset val="1"/>
-          </rPr>
-          <t>Chapman: Chapman-like in Z
-Rect: boxcar
-transcar: from the classic Fortran program</t>
-        </r>
-      </text>
-    </comment>
-  </commentList>
-</comments>
-</file>
-
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="135">
   <si>
     <t>Sim</t>
   </si>
@@ -522,6 +478,9 @@
   </si>
   <si>
     <t>minflux</t>
+  </si>
+  <si>
+    <t>mingaussEv</t>
   </si>
   <si>
     <t>maxIter</t>
@@ -1356,12 +1315,12 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H79"/>
+  <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A44" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B79" activeCellId="1" sqref="C11:H18 B79"/>
+      <selection pane="bottomLeft" activeCell="E55" activeCellId="0" sqref="E55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -1939,7 +1898,7 @@
       </c>
       <c r="F53" s="13"/>
     </row>
-    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="4" t="s">
         <v>65</v>
       </c>
@@ -1959,22 +1918,26 @@
       <c r="C55" s="0"/>
       <c r="D55" s="5"/>
       <c r="E55" s="5" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F55" s="13"/>
     </row>
-    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="38"/>
-      <c r="B56" s="39"/>
-      <c r="C56" s="39"/>
-    </row>
-    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="4" t="s">
+    <row r="56" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="B57" s="0"/>
-      <c r="C57" s="0"/>
-      <c r="F57" s="40"/>
+      <c r="B56" s="0"/>
+      <c r="C56" s="0"/>
+      <c r="D56" s="5"/>
+      <c r="E56" s="5" t="n">
+        <v>800</v>
+      </c>
+      <c r="F56" s="13"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="38"/>
+      <c r="B57" s="39"/>
+      <c r="C57" s="39"/>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="4" t="s">
@@ -1982,7 +1945,7 @@
       </c>
       <c r="B58" s="0"/>
       <c r="C58" s="0"/>
-      <c r="F58" s="41"/>
+      <c r="F58" s="40"/>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="4" t="s">
@@ -1990,7 +1953,7 @@
       </c>
       <c r="B59" s="0"/>
       <c r="C59" s="0"/>
-      <c r="F59" s="42"/>
+      <c r="F59" s="41"/>
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="4" t="s">
@@ -1998,7 +1961,7 @@
       </c>
       <c r="B60" s="0"/>
       <c r="C60" s="0"/>
-      <c r="F60" s="41"/>
+      <c r="F60" s="42"/>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="4" t="s">
@@ -2006,37 +1969,45 @@
       </c>
       <c r="B61" s="0"/>
       <c r="C61" s="0"/>
-      <c r="F61" s="28"/>
+      <c r="F61" s="41"/>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="4"/>
+      <c r="A62" s="4" t="s">
+        <v>72</v>
+      </c>
       <c r="B62" s="0"/>
       <c r="C62" s="0"/>
-      <c r="F62" s="5"/>
+      <c r="F62" s="28"/>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="4" t="s">
-        <v>72</v>
-      </c>
+      <c r="A63" s="4"/>
       <c r="B63" s="0"/>
       <c r="C63" s="0"/>
-      <c r="E63" s="43"/>
       <c r="F63" s="5"/>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="4" t="s">
+        <v>73</v>
+      </c>
       <c r="B64" s="0"/>
       <c r="C64" s="0"/>
+      <c r="E64" s="43"/>
+      <c r="F64" s="5"/>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A65" s="31" t="s">
-        <v>73</v>
-      </c>
-      <c r="B65" s="5" t="s">
+      <c r="B65" s="0"/>
+      <c r="C65" s="0"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="31" t="s">
         <v>74</v>
       </c>
-      <c r="C65" s="5"/>
-    </row>
-    <row r="79" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B66" s="5" t="s">
+        <v>75</v>
+      </c>
+      <c r="C66" s="5"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -2057,10 +2028,10 @@
   </sheetPr>
   <dimension ref="A1:IQ45"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C6" activeCellId="1" sqref="C11:H18 C6"/>
+      <selection pane="bottomLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -2331,7 +2302,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>1</v>
@@ -2590,7 +2561,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="31" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B3" s="46" t="n">
         <v>0</v>
@@ -2849,7 +2820,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="31" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="B4" s="46" t="n">
         <v>0</v>
@@ -3108,7 +3079,7 @@
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="31" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B5" s="4" t="n">
         <v>512</v>
@@ -3367,7 +3338,7 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="47" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B6" s="46" t="n">
         <v>90</v>
@@ -3626,7 +3597,7 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="48" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B7" s="46" t="n">
         <v>9</v>
@@ -3885,7 +3856,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="31" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B8" s="4" t="n">
         <v>1500</v>
@@ -4144,7 +4115,7 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B9" s="49" t="n">
         <v>250</v>
@@ -4403,7 +4374,7 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B10" s="49"/>
       <c r="C10" s="49"/>
@@ -4658,7 +4629,7 @@
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="38" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B11" s="0"/>
       <c r="C11" s="0"/>
@@ -4913,7 +4884,7 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B12" s="50"/>
       <c r="C12" s="0"/>
@@ -5168,7 +5139,7 @@
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="4" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>50</v>
@@ -5427,7 +5398,7 @@
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="51" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B14" s="52" t="n">
         <v>-1</v>
@@ -5686,7 +5657,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="53" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="B15" s="0"/>
       <c r="C15" s="54"/>
@@ -5941,7 +5912,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="53" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B16" s="0"/>
       <c r="C16" s="54"/>
@@ -6196,7 +6167,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="55" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B17" s="56"/>
       <c r="C17" s="57"/>
@@ -6451,7 +6422,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="4" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B18" s="0"/>
       <c r="C18" s="0"/>
@@ -6959,7 +6930,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B20" s="50"/>
       <c r="C20" s="58"/>
@@ -7214,7 +7185,7 @@
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B21" s="50"/>
       <c r="C21" s="58"/>
@@ -7469,7 +7440,7 @@
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="4" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B22" s="0"/>
       <c r="C22" s="0"/>
@@ -7724,7 +7695,7 @@
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="4" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B23" s="0"/>
       <c r="C23" s="0"/>
@@ -7979,7 +7950,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="4" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B24" s="0" t="n">
         <f aca="false">B9*0.9</f>
@@ -8493,7 +8464,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="4" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B26" s="5" t="n">
         <v>15</v>
@@ -8752,7 +8723,7 @@
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="4" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B27" s="5" t="n">
         <v>2</v>
@@ -9016,7 +8987,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="4" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>512</v>
@@ -9027,7 +8998,7 @@
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="4" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>512</v>
@@ -9038,7 +9009,7 @@
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="4" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>1</v>
@@ -9049,7 +9020,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>1</v>
@@ -9060,7 +9031,7 @@
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="4" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B33" s="0"/>
       <c r="C33" s="0"/>
@@ -9072,7 +9043,7 @@
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="4" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B35" s="59" t="n">
         <v>65.1186367</v>
@@ -9083,7 +9054,7 @@
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B36" s="59" t="n">
         <v>-147.432975</v>
@@ -9099,7 +9070,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B38" s="4" t="n">
         <v>77.51</v>
@@ -9110,7 +9081,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="4" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B39" s="4" t="n">
         <v>19.92</v>
@@ -9121,24 +9092,24 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="4" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="4" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9148,7 +9119,7 @@
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="44" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B43" s="60" t="n">
         <f aca="false">(0.0016)^2</f>
@@ -9161,7 +9132,7 @@
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="44" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B44" s="44" t="n">
         <v>1</v>
@@ -9172,7 +9143,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="44" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B45" s="44" t="n">
         <v>1</v>
@@ -9201,448 +9172,17 @@
   </sheetPr>
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="95" zoomScaleNormal="95" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B1" activeCellId="1" sqref="C11:H18 B1"/>
+      <selection pane="bottomLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="21.1224489795918"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.3367346938776"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="11.4387755102041"/>
     <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.5561224489796"/>
-  </cols>
-  <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="4"/>
-      <c r="B1" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C1" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D1" s="4" t="n">
-        <v>2</v>
-      </c>
-      <c r="E1" s="4" t="n">
-        <v>3</v>
-      </c>
-      <c r="F1" s="4" t="n">
-        <v>4</v>
-      </c>
-      <c r="G1" s="4" t="n">
-        <v>5</v>
-      </c>
-      <c r="H1" s="4" t="n">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
-        <v>116</v>
-      </c>
-      <c r="B2" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="C2" s="61" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="D2" s="61" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="E2" s="61" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="F2" s="61" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="G2" s="61" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="H2" s="61" t="n">
-        <v>0.12</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="F3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="G3" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="H3" s="4" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>119</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="B6" s="4" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="C6" s="4" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="D6" s="4" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="E6" s="4" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="F6" s="4" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="G6" s="4" t="n">
-        <v>0.1</v>
-      </c>
-      <c r="H6" s="4" t="n">
-        <v>0.1</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="4" t="s">
-        <v>121</v>
-      </c>
-      <c r="B7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="C7" s="4" t="n">
-        <v>1</v>
-      </c>
-      <c r="D7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="F7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="G7" s="0" t="n">
-        <v>1</v>
-      </c>
-      <c r="H7" s="0" t="n">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="4" t="s">
-        <v>122</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="C8" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="D8" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="E8" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="G8" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="H8" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="C9" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="D9" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="G9" s="4" t="s">
-        <v>125</v>
-      </c>
-      <c r="H9" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="B11" s="0" t="n">
-        <v>10000</v>
-      </c>
-      <c r="C11" s="0" t="n">
-        <v>5000</v>
-      </c>
-      <c r="D11" s="0" t="n">
-        <v>3750</v>
-      </c>
-      <c r="E11" s="0" t="n">
-        <v>2500</v>
-      </c>
-      <c r="F11" s="0" t="n">
-        <v>1000</v>
-      </c>
-      <c r="G11" s="0" t="n">
-        <v>750</v>
-      </c>
-      <c r="H11" s="0" t="n">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
-        <v>127</v>
-      </c>
-      <c r="B12" s="62" t="n">
-        <v>1100000000000</v>
-      </c>
-      <c r="C12" s="62" t="n">
-        <v>900000000000</v>
-      </c>
-      <c r="D12" s="62" t="n">
-        <v>700000000000</v>
-      </c>
-      <c r="E12" s="62" t="n">
-        <v>500000000000</v>
-      </c>
-      <c r="F12" s="62" t="n">
-        <v>225000000000</v>
-      </c>
-      <c r="G12" s="62" t="n">
-        <v>100000000000</v>
-      </c>
-      <c r="H12" s="62" t="n">
-        <v>110000000000</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
-        <v>128</v>
-      </c>
-      <c r="B13" s="0" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="C13" s="0" t="n">
-        <v>0.375</v>
-      </c>
-      <c r="D13" s="0" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="E13" s="0" t="n">
-        <v>0.5</v>
-      </c>
-      <c r="F13" s="0" t="n">
-        <v>0.75</v>
-      </c>
-      <c r="G13" s="0" t="n">
-        <v>0.9</v>
-      </c>
-      <c r="H13" s="0" t="n">
-        <v>1.1</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>129</v>
-      </c>
-      <c r="B14" s="0" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="C14" s="0" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="D14" s="0" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="E14" s="0" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="F14" s="0" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="G14" s="0" t="n">
-        <v>0.8</v>
-      </c>
-      <c r="H14" s="0" t="n">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
-        <v>130</v>
-      </c>
-      <c r="B15" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="C15" s="0" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="D15" s="0" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="E15" s="0" t="n">
-        <v>2.5</v>
-      </c>
-      <c r="F15" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="G15" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="H15" s="0" t="n">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
-        <v>131</v>
-      </c>
-      <c r="B16" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="C16" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="D16" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="E16" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="F16" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="G16" s="0" t="n">
-        <v>4</v>
-      </c>
-      <c r="H16" s="0" t="n">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="s">
-        <v>132</v>
-      </c>
-      <c r="B17" s="0" t="n">
-        <v>7500</v>
-      </c>
-      <c r="C17" s="0" t="n">
-        <v>5500</v>
-      </c>
-      <c r="D17" s="0" t="n">
-        <v>4750</v>
-      </c>
-      <c r="E17" s="0" t="n">
-        <v>4000</v>
-      </c>
-      <c r="F17" s="0" t="n">
-        <v>3000</v>
-      </c>
-      <c r="G17" s="0" t="n">
-        <v>2500</v>
-      </c>
-      <c r="H17" s="0" t="n">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="s">
-        <v>133</v>
-      </c>
-      <c r="B18" s="0" t="n">
-        <v>0.4</v>
-      </c>
-      <c r="C18" s="0" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="D18" s="0" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="E18" s="0" t="n">
-        <v>0.2</v>
-      </c>
-      <c r="F18" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="G18" s="0" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="H18" s="0" t="n">
-        <v>0.145</v>
-      </c>
-    </row>
-    <row r="58" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
-  </headerFooter>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:H18"/>
-  <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C11" activeCellId="0" sqref="C11:H18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.85"/>
-  <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9671,7 +9211,7 @@
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>0</v>
@@ -9697,47 +9237,47 @@
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B3" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C3" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="E3" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="F3" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G3" s="4" t="n">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H3" s="4" t="n">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
     </row>
-    <row r="6" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>0.1</v>
@@ -9761,9 +9301,9 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B7" s="4" t="n">
         <v>1</v>
@@ -9787,139 +9327,139 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>123</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>125</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>10000</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>10000</v>
+        <v>5000</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>10000</v>
+        <v>3750</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>10000</v>
+        <v>2500</v>
       </c>
       <c r="F11" s="0" t="n">
-        <v>10000</v>
+        <v>1000</v>
       </c>
       <c r="G11" s="0" t="n">
-        <v>10000</v>
+        <v>750</v>
       </c>
       <c r="H11" s="0" t="n">
-        <v>10000</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>500</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="B12" s="62" t="n">
         <v>1100000000000</v>
       </c>
       <c r="C12" s="62" t="n">
-        <v>1100000000000</v>
+        <v>900000000000</v>
       </c>
       <c r="D12" s="62" t="n">
-        <v>1100000000000</v>
+        <v>700000000000</v>
       </c>
       <c r="E12" s="62" t="n">
-        <v>1100000000000</v>
+        <v>500000000000</v>
       </c>
       <c r="F12" s="62" t="n">
-        <v>1100000000000</v>
+        <v>225000000000</v>
       </c>
       <c r="G12" s="62" t="n">
-        <v>1100000000000</v>
+        <v>100000000000</v>
       </c>
       <c r="H12" s="62" t="n">
-        <v>1100000000000</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>110000000000</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.25</v>
       </c>
       <c r="C13" s="0" t="n">
-        <v>0.25</v>
+        <v>0.375</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>0.25</v>
+        <v>0.4</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>0.25</v>
+        <v>0.5</v>
       </c>
       <c r="F13" s="0" t="n">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="G13" s="0" t="n">
-        <v>0.25</v>
+        <v>0.9</v>
       </c>
       <c r="H13" s="0" t="n">
-        <v>0.25</v>
+        <v>1.1</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.8</v>
@@ -9943,21 +9483,21 @@
         <v>0.8</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>3</v>
       </c>
       <c r="C15" s="0" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>3</v>
+        <v>2.5</v>
       </c>
       <c r="F15" s="0" t="n">
         <v>3</v>
@@ -9969,9 +9509,9 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>4</v>
@@ -9995,58 +9535,59 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>7500</v>
       </c>
       <c r="C17" s="0" t="n">
-        <v>7500</v>
+        <v>5500</v>
       </c>
       <c r="D17" s="0" t="n">
-        <v>7500</v>
+        <v>4750</v>
       </c>
       <c r="E17" s="0" t="n">
-        <v>7500</v>
+        <v>4000</v>
       </c>
       <c r="F17" s="0" t="n">
-        <v>7500</v>
+        <v>3000</v>
       </c>
       <c r="G17" s="0" t="n">
-        <v>7500</v>
+        <v>2500</v>
       </c>
       <c r="H17" s="0" t="n">
-        <v>7500</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.4</v>
       </c>
       <c r="C18" s="0" t="n">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="D18" s="0" t="n">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="E18" s="0" t="n">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="F18" s="0" t="n">
-        <v>0.4</v>
+        <v>0.15</v>
       </c>
       <c r="G18" s="0" t="n">
-        <v>0.4</v>
+        <v>0.15</v>
       </c>
       <c r="H18" s="0" t="n">
-        <v>0.4</v>
-      </c>
-    </row>
+        <v>0.145</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
table consolidation, text output
</commit_message>
<xml_diff>
--- a/in/2cam_flame.xlsx
+++ b/in/2cam_flame.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="984" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="970" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Sim" sheetId="1" state="visible" r:id="rId2"/>
@@ -37,7 +37,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>1: Use raw data from HST cameras
+          <t xml:space="preserve">1: Use raw data from HST cameras
 0: make an auroral phantom using “TrueArc” parameters below</t>
         </r>
       </text>
@@ -51,7 +51,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Factor of downsampling in energy space</t>
+          <t xml:space="preserve">Factor of downsampling in energy space</t>
         </r>
       </text>
     </comment>
@@ -64,8 +64,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>[nm] for plotting only
-</t>
+          <t xml:space="preserve">[nm] for plotting only</t>
         </r>
       </text>
     </comment>
@@ -78,7 +77,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>none
+          <t xml:space="preserve">none
 bg3</t>
         </r>
       </text>
@@ -92,7 +91,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>1: use dahlgren 2013 eigenprofiles
+          <t xml:space="preserve">1: use dahlgren 2013 eigenprofiles
 0: use locally computed Transcar profiles</t>
         </r>
       </text>
@@ -106,7 +105,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Use this normally</t>
+          <t xml:space="preserve">Use this normally</t>
         </r>
       </text>
     </comment>
@@ -119,7 +118,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Arbitrary: just spread angles across pixels linearly
+          <t xml:space="preserve">Arbitrary: just spread angles across pixels linearly
 Astrometry: calibrated pixels to skymap</t>
         </r>
       </text>
@@ -133,7 +132,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>transcar
+          <t xml:space="preserve">transcar
 arb</t>
         </r>
       </text>
@@ -147,7 +146,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>ArbChapman: User-placed chapman arc(s)
+          <t xml:space="preserve">ArbChapman: User-placed chapman arc(s)
 SmartChapman: two-step JLS algorithm (not yet implemented)
 backproj: using simple inv(L)*d
 tsvd: truncated SVD</t>
@@ -163,7 +162,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>LineLength: To be consistent with definition of Rayleighs</t>
+          <t xml:space="preserve">LineLength: To be consistent with definition of Rayleighs</t>
         </r>
       </text>
     </comment>
@@ -176,7 +175,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Put Z at end for UTC—required!</t>
+          <t xml:space="preserve">Put Z at end for UTC—required!</t>
         </r>
       </text>
     </comment>
@@ -199,7 +198,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>1: use this camera (necessary when computing L)
+          <t xml:space="preserve">1: use this camera (necessary when computing L)
 0: ignore this camera</t>
         </r>
       </text>
@@ -213,7 +212,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>These two options (must) only take effort for “arbitrary” angle mapping!
+          <t xml:space="preserve">These two options (must) only take effort for “arbitrary” angle mapping!
 3.1436km: 88.3 deg
 10km: 86.5 deg
 50km: 76 deg, 30.5 deg fov, 1500km max length</t>
@@ -229,7 +228,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Factor to scale data numbers by (1: keep original data numbers)</t>
+          <t xml:space="preserve">Factor to scale data numbers by (1: keep original data numbers)</t>
         </r>
       </text>
     </comment>
@@ -242,7 +241,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Support width (pixels) for smoothing</t>
+          <t xml:space="preserve">Support width (pixels) for smoothing</t>
         </r>
       </text>
     </comment>
@@ -255,7 +254,7 @@
             <family val="2"/>
             <charset val="1"/>
           </rPr>
-          <t>Photoelectron/data number</t>
+          <t xml:space="preserve">Photoelectron/data number</t>
         </r>
       </text>
     </comment>
@@ -1296,7 +1295,7 @@
   </sheetPr>
   <dimension ref="A1:H80"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="E55" activeCellId="0" sqref="E55"/>
@@ -9148,10 +9147,10 @@
   </sheetPr>
   <dimension ref="A1:H58"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C11" activeCellId="0" sqref="C11"/>
+      <selection pane="bottomLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -9363,13 +9362,13 @@
         <v>10000</v>
       </c>
       <c r="C11" s="0" t="n">
-        <v>5000</v>
+        <v>5250</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>3750</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>2500</v>
+        <v>2200</v>
       </c>
       <c r="F11" s="0" t="n">
         <v>1000</v>

</xml_diff>

<commit_message>
remove seaborn from script, push up to script level
</commit_message>
<xml_diff>
--- a/in/2cam_flame.xlsx
+++ b/in/2cam_flame.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Sim" sheetId="1" state="visible" r:id="rId2"/>
@@ -1267,20 +1267,20 @@
   <dimension ref="A1:F66"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
+      <selection pane="bottomLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="36.4489795918367"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.3418367346939"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.10204081632653"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.56122448979592"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.7551020408163"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5969387755102"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="37.0408163265306"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.4489795918367"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.20918367346939"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.66836734693878"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.265306122449"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.4489795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1505,7 +1505,7 @@
       <c r="C23" s="0"/>
       <c r="F23" s="0"/>
     </row>
-    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="20" t="s">
         <v>37</v>
       </c>
@@ -1631,7 +1631,7 @@
       <c r="C37" s="5"/>
       <c r="F37" s="0"/>
     </row>
-    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="27" t="s">
         <v>49</v>
       </c>
@@ -1901,15 +1901,15 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C13" activeCellId="0" sqref="C13"/>
+      <selection pane="bottomLeft" activeCell="C13" activeCellId="1" sqref="C38 C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="39" width="21.5969387755102"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="39" width="22.9489795918367"/>
-    <col collapsed="false" hidden="false" max="251" min="4" style="39" width="10.530612244898"/>
-    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="39" width="21.9234693877551"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="39" width="23.3265306122449"/>
+    <col collapsed="false" hidden="false" max="251" min="4" style="39" width="10.6938775510204"/>
+    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="10.6938775510204"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9044,13 +9044,13 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="E12" activeCellId="1" sqref="C38 E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.3418367346939"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6377551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.4489795918367"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
reckoning with real coordinates
</commit_message>
<xml_diff>
--- a/in/2cam_flame.xlsx
+++ b/in/2cam_flame.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="987" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="992" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sim" sheetId="1" state="visible" r:id="rId2"/>
@@ -250,7 +250,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="A44" authorId="0">
+    <comment ref="A41" authorId="0">
       <text>
         <r>
           <rPr>
@@ -268,7 +268,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="146" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="131">
   <si>
     <t>Sim</t>
   </si>
@@ -577,12 +577,6 @@
   </si>
   <si>
     <t>nHead16</t>
-  </si>
-  <si>
-    <t>latWGS84</t>
-  </si>
-  <si>
-    <t>lonWGS84</t>
   </si>
   <si>
     <t>Bincl</t>
@@ -953,7 +947,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="57">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1170,10 +1164,6 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1266,7 +1256,7 @@
   </sheetPr>
   <dimension ref="A1:F66"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="C38" activeCellId="0" sqref="C38"/>
@@ -1274,13 +1264,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.5969387755102"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="37.0408163265306"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.4489795918367"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="8.20918367346939"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.66836734693878"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="29.265306122449"/>
-    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.4489795918367"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="25.2448979591837"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="36.5816326530612"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="11.2040816326531"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="7.96428571428571"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="7.56122448979592"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="28.8877551020408"/>
+    <col collapsed="false" hidden="false" max="1025" min="7" style="0" width="11.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1896,20 +1886,20 @@
     <tabColor rgb="FFFFFFFF"/>
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:IQ45"/>
+  <dimension ref="A1:IQ42"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C13" activeCellId="1" sqref="C38 C13"/>
+      <selection pane="bottomLeft" activeCell="A35" activeCellId="0" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="39" width="21.9234693877551"/>
-    <col collapsed="false" hidden="false" max="3" min="2" style="39" width="23.3265306122449"/>
-    <col collapsed="false" hidden="false" max="251" min="4" style="39" width="10.6938775510204"/>
-    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="10.6938775510204"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="39" width="21.5969387755102"/>
+    <col collapsed="false" hidden="false" max="3" min="2" style="39" width="22.9489795918367"/>
+    <col collapsed="false" hidden="false" max="251" min="4" style="39" width="10.530612244898"/>
+    <col collapsed="false" hidden="false" max="1025" min="252" style="0" width="10.530612244898"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8914,110 +8904,83 @@
       <c r="A35" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="B35" s="54" t="n">
-        <v>65.1186367</v>
-      </c>
-      <c r="C35" s="54" t="n">
-        <v>65.12657</v>
+      <c r="B35" s="4" t="n">
+        <v>77.51</v>
+      </c>
+      <c r="C35" s="4" t="n">
+        <v>77.5</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="B36" s="54" t="n">
-        <v>-147.432975</v>
-      </c>
-      <c r="C36" s="54" t="n">
-        <v>-147.496908333</v>
+      <c r="B36" s="4" t="n">
+        <v>19.92</v>
+      </c>
+      <c r="C36" s="4" t="n">
+        <v>19.9</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0"/>
-      <c r="B37" s="0"/>
-      <c r="C37" s="0"/>
+      <c r="A37" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="B38" s="4" t="n">
-        <v>77.51</v>
-      </c>
-      <c r="C38" s="4" t="n">
-        <v>77.5</v>
+        <v>107</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="B39" s="4" t="n">
-        <v>19.92</v>
-      </c>
-      <c r="C39" s="4" t="n">
-        <v>19.9</v>
-      </c>
+      <c r="A39" s="0"/>
+      <c r="B39" s="0"/>
+      <c r="C39" s="0"/>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="4" t="s">
-        <v>107</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="B41" s="4" t="s">
+      <c r="A40" s="39" t="s">
         <v>110</v>
       </c>
-      <c r="C41" s="4" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="0"/>
-      <c r="B42" s="0"/>
-      <c r="C42" s="0"/>
-    </row>
-    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="39" t="s">
-        <v>112</v>
-      </c>
-      <c r="B43" s="55" t="n">
+      <c r="B40" s="54" t="n">
         <f aca="false">(0.0016)^2</f>
         <v>2.56E-006</v>
       </c>
-      <c r="C43" s="55" t="n">
+      <c r="C40" s="54" t="n">
         <f aca="false">(0.0016)^2</f>
         <v>2.56E-006</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="39" t="s">
-        <v>113</v>
-      </c>
-      <c r="B44" s="39" t="n">
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="39" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="C44" s="39" t="n">
+      <c r="C41" s="39" t="n">
         <v>1</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="39" t="s">
-        <v>114</v>
-      </c>
-      <c r="B45" s="39" t="n">
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42" s="39" t="n">
         <v>1</v>
       </c>
-      <c r="C45" s="39" t="n">
+      <c r="C42" s="39" t="n">
         <v>1</v>
       </c>
     </row>
@@ -9044,13 +9007,13 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E12" activeCellId="1" sqref="C38 E12"/>
+      <selection pane="bottomLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.6377551020408"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.4489795918367"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="12.4183673469388"/>
+    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.2040816326531"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9079,33 +9042,33 @@
     </row>
     <row r="2" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="C2" s="56" t="n">
+      <c r="C2" s="55" t="n">
         <v>0.02</v>
       </c>
-      <c r="D2" s="56" t="n">
+      <c r="D2" s="55" t="n">
         <v>0.04</v>
       </c>
-      <c r="E2" s="56" t="n">
+      <c r="E2" s="55" t="n">
         <v>0.06</v>
       </c>
-      <c r="F2" s="56" t="n">
+      <c r="F2" s="55" t="n">
         <v>0.08</v>
       </c>
-      <c r="G2" s="56" t="n">
+      <c r="G2" s="55" t="n">
         <v>0.1</v>
       </c>
-      <c r="H2" s="56" t="n">
+      <c r="H2" s="55" t="n">
         <v>0.12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B3" s="4" t="n">
         <v>1</v>
@@ -9131,21 +9094,21 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="4" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="4" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="B5" s="4"/>
       <c r="C5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="4" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B6" s="4" t="n">
         <v>0.1</v>
@@ -9171,7 +9134,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="4" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B7" s="4" t="n">
         <v>1</v>
@@ -9197,59 +9160,59 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="4" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C8" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="D8" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="H8" s="4" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="4" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D9" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="H9" s="4" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>10000</v>
@@ -9275,33 +9238,33 @@
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>126</v>
-      </c>
-      <c r="B12" s="57" t="n">
+        <v>124</v>
+      </c>
+      <c r="B12" s="56" t="n">
         <v>1100000000000</v>
       </c>
-      <c r="C12" s="57" t="n">
+      <c r="C12" s="56" t="n">
         <v>900000000000</v>
       </c>
-      <c r="D12" s="57" t="n">
+      <c r="D12" s="56" t="n">
         <v>700000000000</v>
       </c>
-      <c r="E12" s="57" t="n">
+      <c r="E12" s="56" t="n">
         <v>500000000000</v>
       </c>
-      <c r="F12" s="57" t="n">
+      <c r="F12" s="56" t="n">
         <v>225000000000</v>
       </c>
-      <c r="G12" s="57" t="n">
+      <c r="G12" s="56" t="n">
         <v>100000000000</v>
       </c>
-      <c r="H12" s="57" t="n">
+      <c r="H12" s="56" t="n">
         <v>110000000000</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.25</v>
@@ -9327,7 +9290,7 @@
     </row>
     <row r="14" customFormat="false" ht="12.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>0.8</v>
@@ -9353,7 +9316,7 @@
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>3</v>
@@ -9379,7 +9342,7 @@
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>4</v>
@@ -9405,7 +9368,7 @@
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>7500</v>
@@ -9431,7 +9394,7 @@
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>0.4</v>

</xml_diff>